<commit_message>
add column to game_nfl, add one week of test schedule
</commit_message>
<xml_diff>
--- a/db/seed/seed.xlsx
+++ b/db/seed/seed.xlsx
@@ -5,14 +5,15 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DavidHu/Desktop/coding/projects/myonlinepool/db/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DavidHu/Desktop/coding/projects/myonlinepool/db/seed/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="5860" windowWidth="31060" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="-2080" yWindow="-20740" windowWidth="35320" windowHeight="19300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="team_nfl" sheetId="2" r:id="rId1"/>
+    <sheet name="test_schedule" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>ARI</t>
   </si>
@@ -324,12 +325,39 @@
   </si>
   <si>
     <t>abbreviation</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>home_id</t>
+  </si>
+  <si>
+    <t>away_id</t>
+  </si>
+  <si>
+    <t>home_score</t>
+  </si>
+  <si>
+    <t>away_score</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>start_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -359,13 +387,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -381,8 +414,29 @@
   <tableColumns count="4">
     <tableColumn id="1" name="city"/>
     <tableColumn id="2" name="name"/>
-    <tableColumn id="4" name="abbreviation" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="abbreviation"/>
     <tableColumn id="3" name="league"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H17" totalsRowShown="0">
+  <autoFilter ref="A1:H17"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Season"/>
+    <tableColumn id="2" name="week"/>
+    <tableColumn id="3" name="home_id"/>
+    <tableColumn id="4" name="away_id"/>
+    <tableColumn id="5" name="home_score">
+      <calculatedColumnFormula>RANDBETWEEN(0, 50)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="away_score">
+      <calculatedColumnFormula>RANDBETWEEN(0, 50)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="completed"/>
+    <tableColumn id="8" name="start_time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,7 +707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1132,4 +1186,502 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2016</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>38</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42621.833333333336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>49</v>
+      </c>
+      <c r="F3">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>32</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42624.541666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2016</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>18</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>42624.541666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2016</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>30</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2016</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>29</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2016</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>38</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>5</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2016</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>39</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2016</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>6</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>36</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2016</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>11</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2016</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>43</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>42624.541666608799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2016</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>26</v>
+      </c>
+      <c r="E14">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>34</v>
+      </c>
+      <c r="F14">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>40</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>42624.666666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2016</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>19</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>42624.854166666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2016</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>9</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>42625.833333333336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2016</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>33</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>42625.833333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add identifier to pool
</commit_message>
<xml_diff>
--- a/db/seed/seed.xlsx
+++ b/db/seed/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2080" yWindow="-20740" windowWidth="35320" windowHeight="19300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-3700" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="team_nfl" sheetId="2" r:id="rId1"/>
@@ -356,7 +356,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -389,14 +389,14 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,12 +1244,12 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>0</v>
+        <f t="shared" ref="E2:F17" ca="1" si="0">RANDBETWEEN(0, 50)</f>
+        <v>9</v>
       </c>
       <c r="F2">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1272,12 +1272,12 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="F3">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>32</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1300,12 +1300,12 @@
         <v>6</v>
       </c>
       <c r="E4">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>27</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
       </c>
       <c r="F4">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>18</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -1328,12 +1328,12 @@
         <v>8</v>
       </c>
       <c r="E5">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>42</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="F5">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>30</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -1356,12 +1356,12 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>17</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="F6">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>29</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -1384,12 +1384,12 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>15</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
       <c r="F7">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1412,12 +1412,12 @@
         <v>14</v>
       </c>
       <c r="E8">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
       <c r="F8">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1440,12 +1440,12 @@
         <v>16</v>
       </c>
       <c r="E9">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="F9">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>39</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -1468,12 +1468,12 @@
         <v>18</v>
       </c>
       <c r="E10">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>17</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="F10">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -1496,12 +1496,12 @@
         <v>20</v>
       </c>
       <c r="E11">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>8</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="F11">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>36</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1524,12 +1524,12 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>25</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
       </c>
       <c r="F12">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>11</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1552,12 +1552,12 @@
         <v>24</v>
       </c>
       <c r="E13">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>26</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="F13">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>43</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1580,12 +1580,12 @@
         <v>26</v>
       </c>
       <c r="E14">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>34</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="F14">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>40</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1608,12 +1608,12 @@
         <v>28</v>
       </c>
       <c r="E15">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="F15">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>19</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -1636,12 +1636,12 @@
         <v>30</v>
       </c>
       <c r="E16">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="F16">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>9</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -1661,15 +1661,15 @@
         <v>31</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>42</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="F17">
-        <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>33</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
make game_nfl store UTC time as start time
</commit_message>
<xml_diff>
--- a/db/seed/seed.xlsx
+++ b/db/seed/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30020" yWindow="-21120" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="team_nfl" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
   <si>
     <t>ARI</t>
   </si>
@@ -339,22 +339,31 @@
     <t>completed</t>
   </si>
   <si>
-    <t>start_time</t>
-  </si>
-  <si>
     <t>Panthers</t>
   </si>
   <si>
     <t>Chargers</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>2016/9/8  20:00:00 EDT</t>
+  </si>
+  <si>
+    <t>2016/9/11 13:00:00 EDT</t>
+  </si>
+  <si>
+    <t>2016/9/11 20:30:00 EDT</t>
+  </si>
+  <si>
+    <t>2016/9/12  20:00:00 EDT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -386,14 +395,14 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -436,7 +445,7 @@
       <calculatedColumnFormula>RANDBETWEEN(0, 50)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="completed"/>
-    <tableColumn id="8" name="start_time" dataDxfId="0"/>
+    <tableColumn id="8" name="start_date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -707,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -793,7 +802,7 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -975,7 +984,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
@@ -1192,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1210,7 @@
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1227,7 +1236,7 @@
         <v>103</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1245,17 +1254,17 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:F17" ca="1" si="0">RANDBETWEEN(0, 50)</f>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
-        <v>42621.833333333336</v>
+      <c r="H2" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1273,17 +1282,17 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>42624.541666666664</v>
+      <c r="H3" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1301,17 +1310,17 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
-        <v>42624.541666666664</v>
+      <c r="H4" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1329,17 +1338,17 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
-        <v>42624.541666608799</v>
+      <c r="H5" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1357,17 +1366,17 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="1">
-        <v>42624.541666608799</v>
+      <c r="H6" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1385,17 +1394,17 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="1">
-        <v>42624.541666608799</v>
+      <c r="H7" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1413,17 +1422,17 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
-        <v>42624.541666608799</v>
+      <c r="H8" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1441,17 +1450,17 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="1">
-        <v>42624.541666608799</v>
+      <c r="H9" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1469,17 +1478,17 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="1">
-        <v>42624.541666608799</v>
+      <c r="H10" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1497,7 +1506,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
@@ -1506,8 +1515,8 @@
       <c r="G11" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="1">
-        <v>42624.541666608799</v>
+      <c r="H11" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1525,17 +1534,17 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="1">
-        <v>42624.541666608799</v>
+      <c r="H12" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1553,17 +1562,17 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="1">
-        <v>42624.541666608799</v>
+      <c r="H13" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1581,17 +1590,17 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="1">
-        <v>42624.666666666664</v>
+      <c r="H14" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1609,17 +1618,17 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
-      </c>
       <c r="G15" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
-        <v>42624.854166666664</v>
+      <c r="H15" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1641,13 +1650,13 @@
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="1">
-        <v>42625.833333333336</v>
+      <c r="H16" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1665,17 +1674,17 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="1">
-        <v>42625.833333333336</v>
+      <c r="H17" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update game_nfl to include spread and line
</commit_message>
<xml_diff>
--- a/db/seed/seed.xlsx
+++ b/db/seed/seed.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="114">
   <si>
     <t>ARI</t>
   </si>
@@ -357,7 +357,16 @@
     <t>2016/9/11 20:30:00 EDT</t>
   </si>
   <si>
-    <t>2016/9/12  20:00:00 EDT</t>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>2016/9/12 20:00:00 EDT</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -431,9 +446,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H17" totalsRowShown="0">
-  <autoFilter ref="A1:H17"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:J17" totalsRowShown="0">
+  <autoFilter ref="A1:J17"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="Season"/>
     <tableColumn id="2" name="week"/>
     <tableColumn id="3" name="home_id"/>
@@ -445,7 +460,13 @@
       <calculatedColumnFormula>RANDBETWEEN(0, 50)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="completed"/>
-    <tableColumn id="8" name="start_date" dataDxfId="0"/>
+    <tableColumn id="8" name="start_date" dataDxfId="2"/>
+    <tableColumn id="9" name="line" dataDxfId="1">
+      <calculatedColumnFormula>RANDBETWEEN(-5, 5) * 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="spread" dataDxfId="0">
+      <calculatedColumnFormula>RANDBETWEEN(0, 20)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1199,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1213,7 +1234,7 @@
     <col min="8" max="8" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1238,8 +1259,14 @@
       <c r="H1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2016</v>
       </c>
@@ -1254,11 +1281,11 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:F17" ca="1" si="0">RANDBETWEEN(0, 50)</f>
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1266,8 +1293,16 @@
       <c r="H2" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f t="shared" ref="I2:I17" ca="1" si="1">RANDBETWEEN(-5, 5) * 100</f>
+        <v>-300</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J17" ca="1" si="2">RANDBETWEEN(0, 20)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -1282,11 +1317,11 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1294,8 +1329,16 @@
       <c r="H3" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -1310,11 +1353,11 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -1322,8 +1365,16 @@
       <c r="H4" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -1338,11 +1389,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -1350,8 +1401,16 @@
       <c r="H5" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" ca="1" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2016</v>
       </c>
@@ -1366,11 +1425,11 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -1378,8 +1437,16 @@
       <c r="H6" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" ca="1" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2016</v>
       </c>
@@ -1394,11 +1461,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1406,8 +1473,16 @@
       <c r="H7" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" ca="1" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -1422,11 +1497,11 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1434,8 +1509,16 @@
       <c r="H8" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" ca="1" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2016</v>
       </c>
@@ -1450,11 +1533,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -1462,8 +1545,16 @@
       <c r="H9" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" ca="1" si="1"/>
+        <v>-400</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -1478,11 +1569,11 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -1490,8 +1581,16 @@
       <c r="H10" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f t="shared" ca="1" si="1"/>
+        <v>-400</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2016</v>
       </c>
@@ -1506,11 +1605,11 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1518,8 +1617,16 @@
       <c r="H11" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <f t="shared" ca="1" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2016</v>
       </c>
@@ -1534,11 +1641,11 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1546,8 +1653,16 @@
       <c r="H12" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f t="shared" ca="1" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -1562,11 +1677,11 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1574,8 +1689,16 @@
       <c r="H13" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f t="shared" ca="1" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -1590,11 +1713,11 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1602,8 +1725,16 @@
       <c r="H14" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <f t="shared" ca="1" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2016</v>
       </c>
@@ -1618,11 +1749,11 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -1630,8 +1761,16 @@
       <c r="H15" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <f t="shared" ca="1" si="1"/>
+        <v>-400</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -1646,20 +1785,28 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2016</v>
       </c>
@@ -1674,17 +1821,30 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add week 2 seeds for schedule
</commit_message>
<xml_diff>
--- a/db/seed/seed.xlsx
+++ b/db/seed/seed.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="113">
   <si>
     <t>ARI</t>
   </si>
@@ -361,9 +361,6 @@
   </si>
   <si>
     <t>line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
   </si>
   <si>
     <t>2016/9/12 20:00:00 EDT</t>
@@ -446,8 +443,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:J17" totalsRowShown="0">
-  <autoFilter ref="A1:J17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:J33" totalsRowShown="0">
+  <autoFilter ref="A1:J33"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Season"/>
     <tableColumn id="2" name="week"/>
@@ -1220,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,12 +1277,12 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:F17" ca="1" si="0">RANDBETWEEN(0, 50)</f>
-        <v>23</v>
+        <f t="shared" ref="E2:F18" ca="1" si="0">RANDBETWEEN(0, 50)</f>
+        <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1294,12 +1291,12 @@
         <v>107</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I17" ca="1" si="1">RANDBETWEEN(-5, 5) * 100</f>
-        <v>-300</v>
+        <f t="shared" ref="I2:I33" ca="1" si="1">RANDBETWEEN(-5, 5) * 100</f>
+        <v>100</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J17" ca="1" si="2">RANDBETWEEN(0, 20)</f>
-        <v>17</v>
+        <f t="shared" ref="J2:J33" ca="1" si="2">RANDBETWEEN(0, 20)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1317,11 +1314,11 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1335,7 +1332,7 @@
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1353,11 +1350,11 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -1367,7 +1364,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>-500</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="2"/>
@@ -1389,11 +1386,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -1403,11 +1400,11 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1425,11 +1422,11 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -1439,11 +1436,11 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1461,11 +1458,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1475,11 +1472,11 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1497,11 +1494,11 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1511,11 +1508,11 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>400</v>
+        <v>-300</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1533,11 +1530,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -1547,11 +1544,11 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v>-400</v>
+        <v>-100</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1569,11 +1566,11 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -1583,7 +1580,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>-400</v>
+        <v>-200</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="2"/>
@@ -1605,11 +1602,11 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1619,11 +1616,11 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1641,11 +1638,11 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1655,11 +1652,11 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
-        <v>300</v>
+        <v>-300</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1677,11 +1674,11 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1691,11 +1688,11 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1713,11 +1710,11 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1727,11 +1724,11 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1749,11 +1746,11 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -1763,11 +1760,11 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="1"/>
-        <v>-400</v>
+        <v>-500</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1785,25 +1782,25 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="1"/>
-        <v>-200</v>
+        <v>200</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1817,34 +1814,605 @@
         <v>31</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2016</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2016</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:F33" ca="1" si="3">RANDBETWEEN(0, 50)</f>
+        <v>24</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2016</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2016</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-300</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2016</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2016</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2016</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-400</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2016</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-300</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2016</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="3"/>
         <v>49</v>
       </c>
-      <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I17">
-        <f t="shared" ca="1" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="J17">
-        <f t="shared" ca="1" si="2"/>
+      <c r="F26">
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2016</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ca="1" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2016</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="3"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G20" t="s">
+      <c r="F28">
+        <f t="shared" ca="1" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2016</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-300</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2016</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ca="1" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ca="1" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2016</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ca="1" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ca="1" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2016</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ca="1" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>